<commit_message>
window size and email message update
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/QuickQuote/QuickQuoteTestData.xlsx
+++ b/binaries/FCfiles/QuickQuote/QuickQuoteTestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="318">
   <si>
     <t>shipmentType</t>
   </si>
@@ -972,6 +972,15 @@
   </si>
   <si>
     <t>51499682</t>
+  </si>
+  <si>
+    <t>51500029</t>
+  </si>
+  <si>
+    <t>10-14-2021</t>
+  </si>
+  <si>
+    <t>FCBTXA1000168</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1016,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="372">
+  <fills count="382">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2864,8 +2873,58 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="365">
+  <borders count="375">
     <border>
       <left/>
       <right/>
@@ -3646,6 +3705,41 @@
         <color auto="1"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
     <border>
       <top style="thin"/>
@@ -4684,7 +4778,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="235">
+  <cellXfs count="240">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -4919,7 +5013,12 @@
     <xf applyBorder="true" applyFill="true" borderId="358" fillId="365" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="360" fillId="367" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="362" fillId="369" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="371" borderId="364" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="364" fillId="371" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="366" fillId="373" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="368" fillId="375" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="370" fillId="377" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="372" fillId="379" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="381" borderId="374" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -5567,8 +5666,8 @@
       <c r="A2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="167" t="s">
-        <v>271</v>
+      <c r="B2" s="236" t="s">
+        <v>316</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>18</v>
@@ -5619,20 +5718,20 @@
       <c r="U2" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="V2" s="166" t="s">
-        <v>270</v>
+      <c r="V2" s="235" t="s">
+        <v>315</v>
       </c>
       <c r="W2" s="171" t="s">
         <v>273</v>
       </c>
-      <c r="X2" s="168" t="s">
+      <c r="X2" s="237" t="s">
         <v>213</v>
       </c>
-      <c r="Y2" s="169" t="s">
-        <v>272</v>
-      </c>
-      <c r="Z2" s="170" t="s">
-        <v>272</v>
+      <c r="Y2" s="238" t="s">
+        <v>317</v>
+      </c>
+      <c r="Z2" s="239" t="s">
+        <v>317</v>
       </c>
       <c r="AA2" s="87" t="s">
         <v>206</v>

</xml_diff>